<commit_message>
no more extra Active column in CommManagement
</commit_message>
<xml_diff>
--- a/ProgramSrc/shelData.xlsx
+++ b/ProgramSrc/shelData.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M25"/>
+  <dimension ref="A1:N25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,60 +441,65 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>Active</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>Name</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>xDegrees</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>yDegrees</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Area1</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>Cost1</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Area2</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>Cost2</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>ResToFlood</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>ResToTyphoon</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>ResToEarthquake</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>Status</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>Remarks</t>
         </is>
@@ -506,42 +511,42 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
           <t>BMLTC Multi-Purpose Bldg and EC</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="D2" t="inlineStr">
         <is>
           <t>14.9185376869108</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="E2" t="inlineStr">
         <is>
           <t>120.766768211462</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>100</t>
-        </is>
-      </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>100</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>200</t>
+          <t>0</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>1000000</t>
+          <t>200</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>1000000</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
@@ -556,10 +561,15 @@
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>Built</t>
-        </is>
-      </c>
-      <c r="M2" t="inlineStr"/>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>Built</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="b">
@@ -567,42 +577,42 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
           <t>F. Mendoza Memorial Elem Sch.</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="D3" t="inlineStr">
         <is>
           <t>14.9176780529243</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
+      <c r="E3" t="inlineStr">
         <is>
           <t>120.767878787289</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>100</t>
-        </is>
-      </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>100</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>200</t>
+          <t>0</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>1000000</t>
+          <t>200</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>1000000</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
@@ -612,15 +622,20 @@
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>Built</t>
-        </is>
-      </c>
-      <c r="M3" t="inlineStr"/>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>Built</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="b">
@@ -628,42 +643,42 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
           <t>Calumpit Sports Complex</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
+      <c r="D4" t="inlineStr">
         <is>
           <t>14.9185209048724</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
+      <c r="E4" t="inlineStr">
         <is>
           <t>120.767571728115</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>100</t>
-        </is>
-      </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>100</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>200</t>
+          <t>0</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>1000000</t>
+          <t>200</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>1000000</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
@@ -678,10 +693,15 @@
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>Built</t>
-        </is>
-      </c>
-      <c r="M4" t="inlineStr"/>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>Built</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="b">
@@ -689,42 +709,42 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
           <t>Gatbuca Basketball Court</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
+      <c r="D5" t="inlineStr">
         <is>
           <t>14.9221390531142</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
+      <c r="E5" t="inlineStr">
         <is>
           <t>120.766774213649</t>
         </is>
       </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>100</t>
-        </is>
-      </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>100</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>200</t>
+          <t>0</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>1000000</t>
+          <t>200</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>1000000</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
@@ -739,10 +759,15 @@
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>Built</t>
-        </is>
-      </c>
-      <c r="M5" t="inlineStr"/>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>Built</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="b">
@@ -750,42 +775,42 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
           <t>San Miguel Evacuation Center</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr">
+      <c r="D6" t="inlineStr">
         <is>
           <t>14.9239360863606</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr">
+      <c r="E6" t="inlineStr">
         <is>
           <t>120.743854227842</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>100</t>
-        </is>
-      </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>100</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>200</t>
+          <t>0</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>1000000</t>
+          <t>200</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>1000000</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
@@ -800,10 +825,15 @@
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>Built</t>
-        </is>
-      </c>
-      <c r="M6" t="inlineStr"/>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>Built</t>
+        </is>
+      </c>
+      <c r="N6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="b">
@@ -811,42 +841,42 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
           <t>Doña Damiana Elem School</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr">
+      <c r="D7" t="inlineStr">
         <is>
           <t>14.9183631788682</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr">
+      <c r="E7" t="inlineStr">
         <is>
           <t>120.74341426756</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>100</t>
-        </is>
-      </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>100</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>200</t>
+          <t>0</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>1000000</t>
+          <t>200</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>1000000</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
@@ -856,15 +886,20 @@
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>Built</t>
-        </is>
-      </c>
-      <c r="M7" t="inlineStr"/>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>Built</t>
+        </is>
+      </c>
+      <c r="N7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="b">
@@ -872,42 +907,42 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
           <t>Danga Dike</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr">
+      <c r="D8" t="inlineStr">
         <is>
           <t>14.9271290793079</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr">
+      <c r="E8" t="inlineStr">
         <is>
           <t>120.75016278348</t>
         </is>
       </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>100</t>
-        </is>
-      </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>100</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>200</t>
+          <t>0</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>1000000</t>
+          <t>200</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>1000000</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
@@ -922,10 +957,15 @@
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>Built</t>
-        </is>
-      </c>
-      <c r="M8" t="inlineStr"/>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>Built</t>
+        </is>
+      </c>
+      <c r="N8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="b">
@@ -933,42 +973,42 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
           <t>Meysulao Multipurpose/E.C.</t>
         </is>
       </c>
-      <c r="C9" t="inlineStr">
+      <c r="D9" t="inlineStr">
         <is>
           <t>14.9059685215204</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr">
+      <c r="E9" t="inlineStr">
         <is>
           <t>120.739306695061</t>
         </is>
       </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>100</t>
-        </is>
-      </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>100</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>200</t>
+          <t>0</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>1000000</t>
+          <t>200</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>1000000</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
@@ -983,10 +1023,15 @@
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>Built</t>
-        </is>
-      </c>
-      <c r="M9" t="inlineStr"/>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>Built</t>
+        </is>
+      </c>
+      <c r="N9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="b">
@@ -994,42 +1039,42 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
           <t xml:space="preserve">Meysulao Dike </t>
         </is>
       </c>
-      <c r="C10" t="inlineStr">
+      <c r="D10" t="inlineStr">
         <is>
           <t>14.9103133008009</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr">
+      <c r="E10" t="inlineStr">
         <is>
           <t>120.738828966419</t>
         </is>
       </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>100</t>
-        </is>
-      </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>100</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>200</t>
+          <t>0</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>1000000</t>
+          <t>200</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>1000000</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
@@ -1044,10 +1089,15 @@
       </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t>Built</t>
-        </is>
-      </c>
-      <c r="M10" t="inlineStr"/>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>Built</t>
+        </is>
+      </c>
+      <c r="N10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="b">
@@ -1055,42 +1105,42 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
           <t>Calizon Dike</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr">
+      <c r="D11" t="inlineStr">
         <is>
           <t>14.9149192538653</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr">
+      <c r="E11" t="inlineStr">
         <is>
           <t>120.749282551866</t>
         </is>
       </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>100</t>
-        </is>
-      </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>100</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>200</t>
+          <t>0</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>1000000</t>
+          <t>200</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>1000000</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
@@ -1105,10 +1155,15 @@
       </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t>Built</t>
-        </is>
-      </c>
-      <c r="M11" t="inlineStr"/>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>Built</t>
+        </is>
+      </c>
+      <c r="N11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="b">
@@ -1116,42 +1171,42 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
           <t>San Marcos Elem. Sch.</t>
         </is>
       </c>
-      <c r="C12" t="inlineStr">
+      <c r="D12" t="inlineStr">
         <is>
           <t>14.8978852342351</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr">
+      <c r="E12" t="inlineStr">
         <is>
           <t>120.778807101888</t>
         </is>
       </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>100</t>
-        </is>
-      </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>100</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>200</t>
+          <t>0</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>1000000</t>
+          <t>200</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>1000000</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
@@ -1161,15 +1216,20 @@
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="L12" t="inlineStr">
         <is>
-          <t>Built</t>
-        </is>
-      </c>
-      <c r="M12" t="inlineStr"/>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M12" t="inlineStr">
+        <is>
+          <t>Built</t>
+        </is>
+      </c>
+      <c r="N12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="b">
@@ -1177,42 +1237,42 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
           <t>San Marcos National H.S.</t>
         </is>
       </c>
-      <c r="C13" t="inlineStr">
+      <c r="D13" t="inlineStr">
         <is>
           <t>14.8938559117996</t>
         </is>
       </c>
-      <c r="D13" t="inlineStr">
+      <c r="E13" t="inlineStr">
         <is>
           <t>120.778052198391</t>
         </is>
       </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>100</t>
-        </is>
-      </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>100</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>200</t>
+          <t>0</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>1000000</t>
+          <t>200</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>1000000</t>
         </is>
       </c>
       <c r="J13" t="inlineStr">
@@ -1222,15 +1282,20 @@
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="L13" t="inlineStr">
         <is>
-          <t>Built</t>
-        </is>
-      </c>
-      <c r="M13" t="inlineStr"/>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M13" t="inlineStr">
+        <is>
+          <t>Built</t>
+        </is>
+      </c>
+      <c r="N13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="b">
@@ -1238,42 +1303,42 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
           <t>GMA Kapuso E.C.</t>
         </is>
       </c>
-      <c r="C14" t="inlineStr">
+      <c r="D14" t="inlineStr">
         <is>
           <t>14.8957602136898</t>
         </is>
       </c>
-      <c r="D14" t="inlineStr">
+      <c r="E14" t="inlineStr">
         <is>
           <t>120.796318926682</t>
         </is>
       </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>100</t>
-        </is>
-      </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>100</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>200</t>
+          <t>0</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>1000000</t>
+          <t>200</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>1000000</t>
         </is>
       </c>
       <c r="J14" t="inlineStr">
@@ -1288,10 +1353,15 @@
       </c>
       <c r="L14" t="inlineStr">
         <is>
-          <t>Built</t>
-        </is>
-      </c>
-      <c r="M14" t="inlineStr"/>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="M14" t="inlineStr">
+        <is>
+          <t>Built</t>
+        </is>
+      </c>
+      <c r="N14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="b">
@@ -1299,42 +1369,42 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
           <t>NV9 Multi-Purpose</t>
         </is>
       </c>
-      <c r="C15" t="inlineStr">
+      <c r="D15" t="inlineStr">
         <is>
           <t>14.8984661105575</t>
         </is>
       </c>
-      <c r="D15" t="inlineStr">
+      <c r="E15" t="inlineStr">
         <is>
           <t>120.765656923103</t>
         </is>
       </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>100</t>
-        </is>
-      </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>100</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>200</t>
+          <t>0</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>1000000</t>
+          <t>200</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>1000000</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
@@ -1349,10 +1419,15 @@
       </c>
       <c r="L15" t="inlineStr">
         <is>
-          <t>Built</t>
-        </is>
-      </c>
-      <c r="M15" t="inlineStr"/>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="M15" t="inlineStr">
+        <is>
+          <t>Built</t>
+        </is>
+      </c>
+      <c r="N15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="b">
@@ -1360,42 +1435,42 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
           <t>Frances E.C.</t>
         </is>
       </c>
-      <c r="C16" t="inlineStr">
+      <c r="D16" t="inlineStr">
         <is>
           <t>14.9194611702998</t>
         </is>
       </c>
-      <c r="D16" t="inlineStr">
+      <c r="E16" t="inlineStr">
         <is>
           <t>120.762172685224</t>
         </is>
       </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>100</t>
-        </is>
-      </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>100</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>200</t>
+          <t>0</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>1000000</t>
+          <t>200</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>1000000</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
@@ -1410,10 +1485,15 @@
       </c>
       <c r="L16" t="inlineStr">
         <is>
-          <t>Built</t>
-        </is>
-      </c>
-      <c r="M16" t="inlineStr"/>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="M16" t="inlineStr">
+        <is>
+          <t>Built</t>
+        </is>
+      </c>
+      <c r="N16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="b">
@@ -1421,42 +1501,42 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
           <t>Balungao E.C.</t>
         </is>
       </c>
-      <c r="C17" t="inlineStr">
+      <c r="D17" t="inlineStr">
         <is>
           <t>14.9148551401837</t>
         </is>
       </c>
-      <c r="D17" t="inlineStr">
+      <c r="E17" t="inlineStr">
         <is>
           <t>120.761492937455</t>
         </is>
       </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>100</t>
-        </is>
-      </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>100</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>200</t>
+          <t>0</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>1000000</t>
+          <t>200</t>
         </is>
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>1000000</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
@@ -1471,10 +1551,15 @@
       </c>
       <c r="L17" t="inlineStr">
         <is>
-          <t>Built</t>
-        </is>
-      </c>
-      <c r="M17" t="inlineStr"/>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="M17" t="inlineStr">
+        <is>
+          <t>Built</t>
+        </is>
+      </c>
+      <c r="N17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="b">
@@ -1482,42 +1567,42 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
           <t>Gugo E.C.</t>
         </is>
       </c>
-      <c r="C18" t="inlineStr">
+      <c r="D18" t="inlineStr">
         <is>
           <t>14.9020620809296</t>
         </is>
       </c>
-      <c r="D18" t="inlineStr">
+      <c r="E18" t="inlineStr">
         <is>
           <t>120.754567377767</t>
         </is>
       </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>100</t>
-        </is>
-      </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>100</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>200</t>
+          <t>0</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>1000000</t>
+          <t>200</t>
         </is>
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>1000000</t>
         </is>
       </c>
       <c r="J18" t="inlineStr">
@@ -1532,10 +1617,15 @@
       </c>
       <c r="L18" t="inlineStr">
         <is>
-          <t>Built</t>
-        </is>
-      </c>
-      <c r="M18" t="inlineStr"/>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="M18" t="inlineStr">
+        <is>
+          <t>Built</t>
+        </is>
+      </c>
+      <c r="N18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="b">
@@ -1543,42 +1633,42 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
           <t>San Marcos E.C.</t>
         </is>
       </c>
-      <c r="C19" t="inlineStr">
+      <c r="D19" t="inlineStr">
         <is>
           <t>14.8977769256005</t>
         </is>
       </c>
-      <c r="D19" t="inlineStr">
+      <c r="E19" t="inlineStr">
         <is>
           <t>120.779698188389</t>
         </is>
       </c>
-      <c r="E19" t="inlineStr">
-        <is>
-          <t>100</t>
-        </is>
-      </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>100</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>200</t>
+          <t>0</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>1000000</t>
+          <t>200</t>
         </is>
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>1000000</t>
         </is>
       </c>
       <c r="J19" t="inlineStr">
@@ -1593,10 +1683,15 @@
       </c>
       <c r="L19" t="inlineStr">
         <is>
-          <t>Built</t>
-        </is>
-      </c>
-      <c r="M19" t="inlineStr"/>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="M19" t="inlineStr">
+        <is>
+          <t>Built</t>
+        </is>
+      </c>
+      <c r="N19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="b">
@@ -1604,42 +1699,42 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
           <t>San Jose E.C.</t>
         </is>
       </c>
-      <c r="C20" t="inlineStr">
+      <c r="D20" t="inlineStr">
         <is>
           <t>14.8832968907295</t>
         </is>
       </c>
-      <c r="D20" t="inlineStr">
+      <c r="E20" t="inlineStr">
         <is>
           <t>120.734404217521</t>
         </is>
       </c>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t>100</t>
-        </is>
-      </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>100</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>200</t>
+          <t>0</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>1000000</t>
+          <t>200</t>
         </is>
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>1000000</t>
         </is>
       </c>
       <c r="J20" t="inlineStr">
@@ -1654,10 +1749,15 @@
       </c>
       <c r="L20" t="inlineStr">
         <is>
-          <t>Built</t>
-        </is>
-      </c>
-      <c r="M20" t="inlineStr"/>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="M20" t="inlineStr">
+        <is>
+          <t>Built</t>
+        </is>
+      </c>
+      <c r="N20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="b">
@@ -1665,42 +1765,42 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
           <t>MEYTO Multi-Purpose/ E.C.</t>
         </is>
       </c>
-      <c r="C21" t="inlineStr">
+      <c r="D21" t="inlineStr">
         <is>
           <t>14.8833047964844</t>
         </is>
       </c>
-      <c r="D21" t="inlineStr">
+      <c r="E21" t="inlineStr">
         <is>
           <t>120.72904705443</t>
         </is>
       </c>
-      <c r="E21" t="inlineStr">
-        <is>
-          <t>100</t>
-        </is>
-      </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>100</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>200</t>
+          <t>0</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>1000000</t>
+          <t>200</t>
         </is>
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>1000000</t>
         </is>
       </c>
       <c r="J21" t="inlineStr">
@@ -1715,10 +1815,15 @@
       </c>
       <c r="L21" t="inlineStr">
         <is>
-          <t>Built</t>
-        </is>
-      </c>
-      <c r="M21" t="inlineStr"/>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="M21" t="inlineStr">
+        <is>
+          <t>Built</t>
+        </is>
+      </c>
+      <c r="N21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="b">
@@ -1726,42 +1831,42 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
           <t>Barangay Hall Bulusan</t>
         </is>
       </c>
-      <c r="C22" t="inlineStr">
+      <c r="D22" t="inlineStr">
         <is>
           <t>14.9104237817507</t>
         </is>
       </c>
-      <c r="D22" t="inlineStr">
+      <c r="E22" t="inlineStr">
         <is>
           <t>120.742556915324</t>
         </is>
       </c>
-      <c r="E22" t="inlineStr">
-        <is>
-          <t>100</t>
-        </is>
-      </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>100</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>200</t>
+          <t>0</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>1000000</t>
+          <t>200</t>
         </is>
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>1000000</t>
         </is>
       </c>
       <c r="J22" t="inlineStr">
@@ -1776,10 +1881,15 @@
       </c>
       <c r="L22" t="inlineStr">
         <is>
-          <t>Built</t>
-        </is>
-      </c>
-      <c r="M22" t="inlineStr"/>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="M22" t="inlineStr">
+        <is>
+          <t>Built</t>
+        </is>
+      </c>
+      <c r="N22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="b">
@@ -1787,42 +1897,42 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
           <t>Brgy. Hall Sta. Lucia</t>
         </is>
       </c>
-      <c r="C23" t="inlineStr">
+      <c r="D23" t="inlineStr">
         <is>
           <t>14.9014927315593</t>
         </is>
       </c>
-      <c r="D23" t="inlineStr">
+      <c r="E23" t="inlineStr">
         <is>
           <t>120.736527735677</t>
         </is>
       </c>
-      <c r="E23" t="inlineStr">
-        <is>
-          <t>100</t>
-        </is>
-      </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>100</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>200</t>
+          <t>0</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>1000000</t>
+          <t>200</t>
         </is>
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>1000000</t>
         </is>
       </c>
       <c r="J23" t="inlineStr">
@@ -1837,10 +1947,15 @@
       </c>
       <c r="L23" t="inlineStr">
         <is>
-          <t>Built</t>
-        </is>
-      </c>
-      <c r="M23" t="inlineStr"/>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="M23" t="inlineStr">
+        <is>
+          <t>Built</t>
+        </is>
+      </c>
+      <c r="N23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="b">
@@ -1848,42 +1963,42 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
           <t>Mun. Covered Court</t>
         </is>
       </c>
-      <c r="C24" t="inlineStr">
+      <c r="D24" t="inlineStr">
         <is>
           <t>14.9142263888355</t>
         </is>
       </c>
-      <c r="D24" t="inlineStr">
+      <c r="E24" t="inlineStr">
         <is>
           <t>120.765260684344</t>
         </is>
       </c>
-      <c r="E24" t="inlineStr">
-        <is>
-          <t>100</t>
-        </is>
-      </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>100</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>200</t>
+          <t>0</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>1000000</t>
+          <t>200</t>
         </is>
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>1000000</t>
         </is>
       </c>
       <c r="J24" t="inlineStr">
@@ -1898,10 +2013,15 @@
       </c>
       <c r="L24" t="inlineStr">
         <is>
-          <t>Built</t>
-        </is>
-      </c>
-      <c r="M24" t="inlineStr"/>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="M24" t="inlineStr">
+        <is>
+          <t>Built</t>
+        </is>
+      </c>
+      <c r="N24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="b">
@@ -1909,24 +2029,24 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
           <t>testAdd</t>
         </is>
       </c>
-      <c r="C25" t="inlineStr">
+      <c r="D25" t="inlineStr">
         <is>
           <t>0.0</t>
         </is>
       </c>
-      <c r="D25" t="inlineStr">
+      <c r="E25" t="inlineStr">
         <is>
           <t>0.0</t>
         </is>
       </c>
-      <c r="E25" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
       <c r="F25" t="inlineStr">
         <is>
           <t>0</t>
@@ -1944,7 +2064,7 @@
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="J25" t="inlineStr">
@@ -1959,10 +2079,15 @@
       </c>
       <c r="L25" t="inlineStr">
         <is>
-          <t>Built</t>
-        </is>
-      </c>
-      <c r="M25" t="inlineStr"/>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="M25" t="inlineStr">
+        <is>
+          <t>Built</t>
+        </is>
+      </c>
+      <c r="N25" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
no more Active column in shelter also
</commit_message>
<xml_diff>
--- a/ProgramSrc/shelData.xlsx
+++ b/ProgramSrc/shelData.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N25"/>
+  <dimension ref="A1:M23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,65 +441,60 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Active</t>
+          <t>Name</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Name</t>
+          <t>xDegrees</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>xDegrees</t>
+          <t>yDegrees</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>yDegrees</t>
+          <t>Area1</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Area1</t>
+          <t>Cost1</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>Cost1</t>
+          <t>Area2</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>Area2</t>
+          <t>Cost2</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>Cost2</t>
+          <t>ResToFlood</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>ResToFlood</t>
+          <t>ResToTyphoon</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>ResToTyphoon</t>
+          <t>ResToEarthquake</t>
         </is>
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
-          <t>ResToEarthquake</t>
+          <t>Status</t>
         </is>
       </c>
       <c r="M1" s="1" t="inlineStr">
-        <is>
-          <t>Status</t>
-        </is>
-      </c>
-      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>Remarks</t>
         </is>
@@ -511,329 +506,304 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>BMLTC Multi-Purpose Bldg and EC</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>BMLTC Multi-Purpose Bldg and EC</t>
+          <t>14.9185376869108</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>14.9185376869108</t>
+          <t>120.766768211462</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>120.766768211462</t>
+          <t>1641</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>100</t>
+          <t>0</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>3282</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>200</t>
+          <t>98460000</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>1000000</t>
+          <t>True</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>True</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>True</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="M2" t="inlineStr">
-        <is>
-          <t>Built</t>
-        </is>
-      </c>
-      <c r="N2" t="inlineStr"/>
+          <t>Built</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
+          <t>F. Mendoza Memorial Elem Sch.</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>14.9176780529243</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>120.767878787289</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>1671</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>3342</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>100260000</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
           <t>False</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>F. Mendoza Memorial Elem Sch.</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>14.9176780529243</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>120.767878787289</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>100</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>200</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>1000000</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="M3" t="inlineStr">
-        <is>
-          <t>Built</t>
-        </is>
-      </c>
-      <c r="N3" t="inlineStr"/>
+          <t>Built</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>Calumpit Sports Complex</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Calumpit Sports Complex</t>
+          <t>14.9185209048724</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>14.9185209048724</t>
+          <t>120.767571728115</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>120.767571728115</t>
+          <t>947</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>100</t>
+          <t>0</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1894</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>200</t>
+          <t>56820000</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>1000000</t>
+          <t>True</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>True</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>True</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="M4" t="inlineStr">
-        <is>
-          <t>Built</t>
-        </is>
-      </c>
-      <c r="N4" t="inlineStr"/>
+          <t>Built</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>Gatbuca Basketball Court</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Gatbuca Basketball Court</t>
+          <t>14.9221390531142</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>14.9221390531142</t>
+          <t>120.766774213649</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>120.766774213649</t>
+          <t>376</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>100</t>
+          <t>0</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>752</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>200</t>
+          <t>22560000</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>1000000</t>
+          <t>True</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>True</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>True</t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="M5" t="inlineStr">
-        <is>
-          <t>Built</t>
-        </is>
-      </c>
-      <c r="N5" t="inlineStr"/>
+          <t>Built</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>San Miguel Meysulao High School</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>San Miguel Evacuation Center</t>
+          <t>14.9167991010101</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>14.9239360863606</t>
+          <t>120.742941581954</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>120.743854227842</t>
+          <t>3464</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>100</t>
+          <t>0</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>6928</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>200</t>
+          <t>207840000</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>1000000</t>
+          <t>True</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>True</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>True</t>
         </is>
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="M6" t="inlineStr">
-        <is>
-          <t>Built</t>
-        </is>
-      </c>
-      <c r="N6" t="inlineStr"/>
+          <t>Built</t>
+        </is>
+      </c>
+      <c r="M6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="b">
@@ -841,65 +811,60 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>Doña Damiana Elem School</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Doña Damiana Elem School</t>
+          <t>14.917701586824</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>14.9183631788682</t>
+          <t>120.743048619728</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>120.74341426756</t>
+          <t>3135</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>100</t>
+          <t>0</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>6270</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>200</t>
+          <t>188100000</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>1000000</t>
+          <t>True</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>True</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>False</t>
         </is>
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="M7" t="inlineStr">
-        <is>
-          <t>Built</t>
-        </is>
-      </c>
-      <c r="N7" t="inlineStr"/>
+          <t>Built</t>
+        </is>
+      </c>
+      <c r="M7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="b">
@@ -907,131 +872,121 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
+          <t>Danga Dike</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>14.9271290793079</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>120.75016278348</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>126</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>252</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>7560000</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
           <t>False</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>Danga Dike</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>14.9271290793079</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>120.75016278348</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>100</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>200</t>
-        </is>
-      </c>
-      <c r="I8" t="inlineStr">
-        <is>
-          <t>1000000</t>
-        </is>
-      </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>False</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>False</t>
         </is>
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="M8" t="inlineStr">
-        <is>
-          <t>Built</t>
-        </is>
-      </c>
-      <c r="N8" t="inlineStr"/>
+          <t>Built</t>
+        </is>
+      </c>
+      <c r="M8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>Meysulao Multipurpose/E.C.</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Meysulao Multipurpose/E.C.</t>
+          <t>14.905513184046</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>14.9059685215204</t>
+          <t>120.739161033176</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>120.739306695061</t>
+          <t>100</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>100</t>
+          <t>0</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>200</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>200</t>
+          <t>6000000</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>1000000</t>
+          <t>True</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>True</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>True</t>
         </is>
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="M9" t="inlineStr">
-        <is>
-          <t>Built</t>
-        </is>
-      </c>
-      <c r="N9" t="inlineStr"/>
+          <t>Built</t>
+        </is>
+      </c>
+      <c r="M9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="b">
@@ -1039,65 +994,60 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
+          <t>Calizon Dike</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>14.9136800407707</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>120.755871075221</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>126</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>252</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>7560000</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
           <t>False</t>
         </is>
       </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Meysulao Dike </t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>14.9103133008009</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>120.738828966419</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>100</t>
-        </is>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t>200</t>
-        </is>
-      </c>
-      <c r="I10" t="inlineStr">
-        <is>
-          <t>1000000</t>
-        </is>
-      </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>False</t>
         </is>
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>False</t>
         </is>
       </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="M10" t="inlineStr">
-        <is>
-          <t>Built</t>
-        </is>
-      </c>
-      <c r="N10" t="inlineStr"/>
+          <t>Built</t>
+        </is>
+      </c>
+      <c r="M10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="b">
@@ -1105,65 +1055,60 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>San Marcos Elem. Sch.</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Calizon Dike</t>
+          <t>14.8978852342351</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>14.9149192538653</t>
+          <t>120.778807101888</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>120.749282551866</t>
+          <t>1147</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>100</t>
+          <t>0</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2294</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>200</t>
+          <t>68820000</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>1000000</t>
+          <t>True</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>True</t>
         </is>
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>False</t>
         </is>
       </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="M11" t="inlineStr">
-        <is>
-          <t>Built</t>
-        </is>
-      </c>
-      <c r="N11" t="inlineStr"/>
+          <t>Built</t>
+        </is>
+      </c>
+      <c r="M11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="b">
@@ -1171,197 +1116,182 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>San Marcos National H.S.</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>San Marcos Elem. Sch.</t>
+          <t>14.8933901983676</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>14.8978852342351</t>
+          <t>120.777840587943</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>120.778807101888</t>
+          <t>6353</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>100</t>
+          <t>0</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>12706</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>200</t>
+          <t>381180000</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>1000000</t>
+          <t>True</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>True</t>
         </is>
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>False</t>
         </is>
       </c>
       <c r="L12" t="inlineStr">
         <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="M12" t="inlineStr">
-        <is>
-          <t>Built</t>
-        </is>
-      </c>
-      <c r="N12" t="inlineStr"/>
+          <t>Built</t>
+        </is>
+      </c>
+      <c r="M12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>GMA Kapuso E.C.</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>San Marcos National H.S.</t>
+          <t>14.8930053477281</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>14.8938559117996</t>
+          <t>120.799658008805</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>120.778052198391</t>
+          <t>200</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>100</t>
+          <t>0</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>400</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>200</t>
+          <t>12000000</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>1000000</t>
+          <t>True</t>
         </is>
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>True</t>
         </is>
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>True</t>
         </is>
       </c>
       <c r="L13" t="inlineStr">
         <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="M13" t="inlineStr">
-        <is>
-          <t>Built</t>
-        </is>
-      </c>
-      <c r="N13" t="inlineStr"/>
+          <t>Built</t>
+        </is>
+      </c>
+      <c r="M13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>NV9 Multi-Purpose</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>GMA Kapuso E.C.</t>
+          <t>14.8980360749457</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>14.8957602136898</t>
+          <t>120.764234222054</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>120.796318926682</t>
+          <t>2513</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>100</t>
+          <t>0</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>5026</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>200</t>
+          <t>150780000</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>1000000</t>
+          <t>True</t>
         </is>
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>True</t>
         </is>
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>True</t>
         </is>
       </c>
       <c r="L14" t="inlineStr">
         <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="M14" t="inlineStr">
-        <is>
-          <t>Built</t>
-        </is>
-      </c>
-      <c r="N14" t="inlineStr"/>
+          <t>Built</t>
+        </is>
+      </c>
+      <c r="M14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="b">
@@ -1369,725 +1299,548 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>Frances E.C.</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>NV9 Multi-Purpose</t>
+          <t>14.9194611702998</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>14.8984661105575</t>
+          <t>120.762172685224</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>120.765656923103</t>
+          <t>150</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>100</t>
+          <t>0</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>300</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>200</t>
+          <t>9000000</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>1000000</t>
+          <t>True</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>True</t>
         </is>
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>True</t>
         </is>
       </c>
       <c r="L15" t="inlineStr">
         <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="M15" t="inlineStr">
-        <is>
-          <t>Built</t>
-        </is>
-      </c>
-      <c r="N15" t="inlineStr"/>
+          <t>Built</t>
+        </is>
+      </c>
+      <c r="M15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>Balungao E.C.</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Frances E.C.</t>
+          <t>14.9148551401837</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>14.9194611702998</t>
+          <t>120.761492937455</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>120.762172685224</t>
+          <t>216</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>100</t>
+          <t>0</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>432</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>200</t>
+          <t>12960000</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>1000000</t>
+          <t>True</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>True</t>
         </is>
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>True</t>
         </is>
       </c>
       <c r="L16" t="inlineStr">
         <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="M16" t="inlineStr">
-        <is>
-          <t>Built</t>
-        </is>
-      </c>
-      <c r="N16" t="inlineStr"/>
+          <t>Built</t>
+        </is>
+      </c>
+      <c r="M16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>Gugo E.C.</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Balungao E.C.</t>
+          <t>14.9013032539823</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>14.9148551401837</t>
+          <t>120.754718122165</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>120.761492937455</t>
+          <t>336</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>100</t>
+          <t>0</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>672</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>200</t>
+          <t>20160000</t>
         </is>
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>1000000</t>
+          <t>True</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>True</t>
         </is>
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>True</t>
         </is>
       </c>
       <c r="L17" t="inlineStr">
         <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="M17" t="inlineStr">
-        <is>
-          <t>Built</t>
-        </is>
-      </c>
-      <c r="N17" t="inlineStr"/>
+          <t>Built</t>
+        </is>
+      </c>
+      <c r="M17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>San Marcos E.C.</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Gugo E.C.</t>
+          <t>14.8976681596682</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>14.9020620809296</t>
+          <t>120.779685551006</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>120.754567377767</t>
+          <t>40</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>100</t>
+          <t>0</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>80</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>200</t>
+          <t>2400000</t>
         </is>
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>1000000</t>
+          <t>True</t>
         </is>
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>True</t>
         </is>
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>True</t>
         </is>
       </c>
       <c r="L18" t="inlineStr">
         <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="M18" t="inlineStr">
-        <is>
-          <t>Built</t>
-        </is>
-      </c>
-      <c r="N18" t="inlineStr"/>
+          <t>Built</t>
+        </is>
+      </c>
+      <c r="M18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>San Jose E.C.</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>San Marcos E.C.</t>
+          <t>14.8832975084056</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>14.8977769256005</t>
+          <t>120.734533125581</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>120.779698188389</t>
+          <t>268</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>100</t>
+          <t>0</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>536</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>200</t>
+          <t>16080000</t>
         </is>
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>1000000</t>
+          <t>True</t>
         </is>
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>True</t>
         </is>
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>True</t>
         </is>
       </c>
       <c r="L19" t="inlineStr">
         <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="M19" t="inlineStr">
-        <is>
-          <t>Built</t>
-        </is>
-      </c>
-      <c r="N19" t="inlineStr"/>
+          <t>Built</t>
+        </is>
+      </c>
+      <c r="M19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>MEYTO Multi-Purpose/ E.C.</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>San Jose E.C.</t>
+          <t>14.8833047964844</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>14.8832968907295</t>
+          <t>120.72904705443</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>120.734404217521</t>
+          <t>142</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>100</t>
+          <t>0</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>284</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>200</t>
+          <t>8520000</t>
         </is>
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>1000000</t>
+          <t>True</t>
         </is>
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>True</t>
         </is>
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>True</t>
         </is>
       </c>
       <c r="L20" t="inlineStr">
         <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="M20" t="inlineStr">
-        <is>
-          <t>Built</t>
-        </is>
-      </c>
-      <c r="N20" t="inlineStr"/>
+          <t>Built</t>
+        </is>
+      </c>
+      <c r="M20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>Barangay Hall Bulusan</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>MEYTO Multi-Purpose/ E.C.</t>
+          <t>14.9087960788938</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>14.8833047964844</t>
+          <t>120.742261855893</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>120.72904705443</t>
+          <t>700</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>100</t>
+          <t>0</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1400</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>200</t>
+          <t>42000000</t>
         </is>
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>1000000</t>
+          <t>True</t>
         </is>
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>True</t>
         </is>
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>True</t>
         </is>
       </c>
       <c r="L21" t="inlineStr">
         <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="M21" t="inlineStr">
-        <is>
-          <t>Built</t>
-        </is>
-      </c>
-      <c r="N21" t="inlineStr"/>
+          <t>Built</t>
+        </is>
+      </c>
+      <c r="M21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>Brgy. Hall Sta. Lucia</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Barangay Hall Bulusan</t>
+          <t>14.8995538574762</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>14.9104237817507</t>
+          <t>120.737428917917</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>120.742556915324</t>
+          <t>150</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>100</t>
+          <t>0</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>300</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>200</t>
+          <t>9000000</t>
         </is>
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>1000000</t>
+          <t>True</t>
         </is>
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>True</t>
         </is>
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>True</t>
         </is>
       </c>
       <c r="L22" t="inlineStr">
         <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="M22" t="inlineStr">
-        <is>
-          <t>Built</t>
-        </is>
-      </c>
-      <c r="N22" t="inlineStr"/>
+          <t>Built</t>
+        </is>
+      </c>
+      <c r="M22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>Mun. Covered Court</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Brgy. Hall Sta. Lucia</t>
+          <t>14.9141384055205</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>14.9014927315593</t>
+          <t>120.764788274642</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>120.736527735677</t>
+          <t>713</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>100</t>
+          <t>0</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1426</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>200</t>
+          <t>42780000</t>
         </is>
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>1000000</t>
+          <t>True</t>
         </is>
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>True</t>
         </is>
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>True</t>
         </is>
       </c>
       <c r="L23" t="inlineStr">
         <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="M23" t="inlineStr">
-        <is>
-          <t>Built</t>
-        </is>
-      </c>
-      <c r="N23" t="inlineStr"/>
-    </row>
-    <row r="24">
-      <c r="A24" t="b">
-        <v>0</v>
-      </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
-      </c>
-      <c r="C24" t="inlineStr">
-        <is>
-          <t>Mun. Covered Court</t>
-        </is>
-      </c>
-      <c r="D24" t="inlineStr">
-        <is>
-          <t>14.9142263888355</t>
-        </is>
-      </c>
-      <c r="E24" t="inlineStr">
-        <is>
-          <t>120.765260684344</t>
-        </is>
-      </c>
-      <c r="F24" t="inlineStr">
-        <is>
-          <t>100</t>
-        </is>
-      </c>
-      <c r="G24" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="H24" t="inlineStr">
-        <is>
-          <t>200</t>
-        </is>
-      </c>
-      <c r="I24" t="inlineStr">
-        <is>
-          <t>1000000</t>
-        </is>
-      </c>
-      <c r="J24" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="K24" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="L24" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="M24" t="inlineStr">
-        <is>
-          <t>Built</t>
-        </is>
-      </c>
-      <c r="N24" t="inlineStr"/>
-    </row>
-    <row r="25">
-      <c r="A25" t="b">
-        <v>0</v>
-      </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
-      </c>
-      <c r="C25" t="inlineStr">
-        <is>
-          <t>testAdd</t>
-        </is>
-      </c>
-      <c r="D25" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="E25" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="F25" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="G25" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="H25" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="I25" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="J25" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="K25" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="L25" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="M25" t="inlineStr">
-        <is>
-          <t>Built</t>
-        </is>
-      </c>
-      <c r="N25" t="inlineStr"/>
+          <t>Built</t>
+        </is>
+      </c>
+      <c r="M23" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
working preview in dashborad
</commit_message>
<xml_diff>
--- a/ProgramSrc/shelData.xlsx
+++ b/ProgramSrc/shelData.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M23"/>
+  <dimension ref="A1:M16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -502,26 +502,26 @@
     </row>
     <row r="2">
       <c r="A2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>wdw</t>
+          <t>San Miguel Meysulao High School</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>14.9185376869108</t>
+          <t>14.9167991010101</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>120.786768211462</t>
+          <t>120.742941581954</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>1641</t>
+          <t>3464</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -531,12 +531,12 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>3282</t>
+          <t>6928</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>98460000</t>
+          <t>207840000</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
@@ -556,33 +556,33 @@
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>Damaged</t>
+          <t>Built</t>
         </is>
       </c>
       <c r="M2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>F. Mendoza Memorial Elem Sch.</t>
+          <t>Danga Dike</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>14.9176780529243</t>
+          <t>14.9271290793079</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>120.767878787289</t>
+          <t>120.75016278348</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>1671</t>
+          <t>126</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -592,22 +592,22 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>3342</t>
+          <t>252</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>100260000</t>
+          <t>7560000</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
@@ -617,33 +617,33 @@
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>Built</t>
+          <t>Partially Built</t>
         </is>
       </c>
       <c r="M3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Calumpit Sports Complex</t>
+          <t>San Marcos Elem. Sch.</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>14.9185209048724</t>
+          <t>14.8978852342351</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>120.767571728115</t>
+          <t>120.778807101888</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>947</t>
+          <t>1147</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -653,12 +653,12 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>1894</t>
+          <t>2294</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>56820000</t>
+          <t>68820000</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
@@ -673,12 +673,12 @@
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>Partially Built</t>
+          <t>Built</t>
         </is>
       </c>
       <c r="M4" t="inlineStr"/>
@@ -689,22 +689,22 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Gatbuca Basketball Court</t>
+          <t>San Marcos National H.S.</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>14.9221390531142</t>
+          <t>14.8933901983676</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>120.766774213649</t>
+          <t>120.777840587943</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>376</t>
+          <t>6353</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -714,12 +714,12 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>752</t>
+          <t>12706</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>22560000</t>
+          <t>381180000</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
@@ -734,7 +734,7 @@
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
@@ -750,22 +750,22 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>San Miguel Meysulao High School</t>
+          <t>GMA Kapuso E.C.</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>14.9167991010101</t>
+          <t>14.8930053477281</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>120.742941581954</t>
+          <t>120.799658008805</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>3464</t>
+          <t>200</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -775,58 +775,58 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>6928</t>
+          <t>400</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>207840000</t>
+          <t>12000000</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>Built</t>
+          <t>Damaged</t>
         </is>
       </c>
       <c r="M6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Doña Damiana Elem School</t>
+          <t>NV9 Multi-Purpose</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>14.917701586824</t>
+          <t>14.8980360749457</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>120.743048619728</t>
+          <t>120.764234222054</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>3135</t>
+          <t>2513</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -836,12 +836,12 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>6270</t>
+          <t>5026</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>188100000</t>
+          <t>150780000</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
@@ -856,7 +856,7 @@
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>True</t>
         </is>
       </c>
       <c r="L7" t="inlineStr">
@@ -872,22 +872,22 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Danga Dike</t>
+          <t>Frances E.C.</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>14.9271290793079</t>
+          <t>14.9194611702998</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>120.75016278348</t>
+          <t>120.762172685224</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>126</t>
+          <t>150</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -897,27 +897,27 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>252</t>
+          <t>300</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>7560000</t>
+          <t>9000000</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>True</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>True</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>True</t>
         </is>
       </c>
       <c r="L8" t="inlineStr">
@@ -933,22 +933,22 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Meysulao Multipurpose/E.C.</t>
+          <t>Balungao E.C.</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>14.905513184046</t>
+          <t>14.9148551401837</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>120.739161033176</t>
+          <t>120.761492937455</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>100</t>
+          <t>216</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -958,12 +958,12 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>200</t>
+          <t>432</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>6000000</t>
+          <t>12960000</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
@@ -994,22 +994,22 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Calizon Dike</t>
+          <t>Gugo E.C.</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>14.9136800407707</t>
+          <t>14.9013032539823</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>120.755871075221</t>
+          <t>120.754718122165</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>126</t>
+          <t>336</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -1019,27 +1019,27 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>252</t>
+          <t>672</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>7560000</t>
+          <t>20160000</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>True</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>True</t>
         </is>
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>True</t>
         </is>
       </c>
       <c r="L10" t="inlineStr">
@@ -1055,22 +1055,22 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>San Marcos Elem. Sch.</t>
+          <t>San Marcos E.C.</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>14.8978852342351</t>
+          <t>14.8976681596682</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>120.778807101888</t>
+          <t>120.779685551006</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>1147</t>
+          <t>40</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -1080,12 +1080,12 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>2294</t>
+          <t>80</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>68820000</t>
+          <t>2400000</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
@@ -1100,7 +1100,7 @@
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>True</t>
         </is>
       </c>
       <c r="L11" t="inlineStr">
@@ -1116,22 +1116,22 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>San Marcos National H.S.</t>
+          <t>San Jose E.C.</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>14.8933901983676</t>
+          <t>14.8832975084056</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>120.777840587943</t>
+          <t>120.734533125581</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>6353</t>
+          <t>268</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -1141,12 +1141,12 @@
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>12706</t>
+          <t>536</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>381180000</t>
+          <t>16080000</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
@@ -1161,7 +1161,7 @@
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>True</t>
         </is>
       </c>
       <c r="L12" t="inlineStr">
@@ -1177,22 +1177,22 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>GMA Kapuso E.C.</t>
+          <t>MEYTO Multi-Purpose/ E.C.</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>14.8930053477281</t>
+          <t>14.8833047964844</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>120.799658008805</t>
+          <t>120.72904705443</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>200</t>
+          <t>142</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -1202,58 +1202,58 @@
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>400</t>
+          <t>284</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>12000000</t>
+          <t>8520000</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>True</t>
         </is>
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>True</t>
         </is>
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>True</t>
         </is>
       </c>
       <c r="L13" t="inlineStr">
         <is>
-          <t>Damaged</t>
+          <t>Built</t>
         </is>
       </c>
       <c r="M13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>NV9 Multi-Purpose</t>
+          <t>Barangay Hall Bulusan</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>14.8980360749457</t>
+          <t>14.9087960788938</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>120.764234222054</t>
+          <t>120.742261855893</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>2513</t>
+          <t>700</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -1263,12 +1263,12 @@
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>5026</t>
+          <t>1400</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>150780000</t>
+          <t>42000000</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
@@ -1299,17 +1299,17 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Frances E.C.</t>
+          <t>Brgy. Hall Sta. Lucia</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>14.9194611702998</t>
+          <t>14.8995538574762</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>120.762172685224</t>
+          <t>120.737428917917</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -1356,26 +1356,26 @@
     </row>
     <row r="16">
       <c r="A16" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Balungao E.C.</t>
+          <t>Mun. Covered Court</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>14.9148551401837</t>
+          <t>14.9141384055205</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>120.761492937455</t>
+          <t>120.764788274642</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>216</t>
+          <t>713</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -1385,12 +1385,12 @@
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>432</t>
+          <t>1426</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>12960000</t>
+          <t>42780000</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
@@ -1414,433 +1414,6 @@
         </is>
       </c>
       <c r="M16" t="inlineStr"/>
-    </row>
-    <row r="17">
-      <c r="A17" t="b">
-        <v>0</v>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>Gugo E.C.</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>14.9013032539823</t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>120.754718122165</t>
-        </is>
-      </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>336</t>
-        </is>
-      </c>
-      <c r="F17" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="G17" t="inlineStr">
-        <is>
-          <t>672</t>
-        </is>
-      </c>
-      <c r="H17" t="inlineStr">
-        <is>
-          <t>20160000</t>
-        </is>
-      </c>
-      <c r="I17" t="inlineStr">
-        <is>
-          <t>True</t>
-        </is>
-      </c>
-      <c r="J17" t="inlineStr">
-        <is>
-          <t>True</t>
-        </is>
-      </c>
-      <c r="K17" t="inlineStr">
-        <is>
-          <t>True</t>
-        </is>
-      </c>
-      <c r="L17" t="inlineStr">
-        <is>
-          <t>Built</t>
-        </is>
-      </c>
-      <c r="M17" t="inlineStr"/>
-    </row>
-    <row r="18">
-      <c r="A18" t="b">
-        <v>0</v>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>San Marcos E.C.</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>14.8976681596682</t>
-        </is>
-      </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>120.779685551006</t>
-        </is>
-      </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>40</t>
-        </is>
-      </c>
-      <c r="F18" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="G18" t="inlineStr">
-        <is>
-          <t>80</t>
-        </is>
-      </c>
-      <c r="H18" t="inlineStr">
-        <is>
-          <t>2400000</t>
-        </is>
-      </c>
-      <c r="I18" t="inlineStr">
-        <is>
-          <t>True</t>
-        </is>
-      </c>
-      <c r="J18" t="inlineStr">
-        <is>
-          <t>True</t>
-        </is>
-      </c>
-      <c r="K18" t="inlineStr">
-        <is>
-          <t>True</t>
-        </is>
-      </c>
-      <c r="L18" t="inlineStr">
-        <is>
-          <t>Built</t>
-        </is>
-      </c>
-      <c r="M18" t="inlineStr"/>
-    </row>
-    <row r="19">
-      <c r="A19" t="b">
-        <v>0</v>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>San Jose E.C.</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>14.8832975084056</t>
-        </is>
-      </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>120.734533125581</t>
-        </is>
-      </c>
-      <c r="E19" t="inlineStr">
-        <is>
-          <t>268</t>
-        </is>
-      </c>
-      <c r="F19" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="G19" t="inlineStr">
-        <is>
-          <t>536</t>
-        </is>
-      </c>
-      <c r="H19" t="inlineStr">
-        <is>
-          <t>16080000</t>
-        </is>
-      </c>
-      <c r="I19" t="inlineStr">
-        <is>
-          <t>True</t>
-        </is>
-      </c>
-      <c r="J19" t="inlineStr">
-        <is>
-          <t>True</t>
-        </is>
-      </c>
-      <c r="K19" t="inlineStr">
-        <is>
-          <t>True</t>
-        </is>
-      </c>
-      <c r="L19" t="inlineStr">
-        <is>
-          <t>Built</t>
-        </is>
-      </c>
-      <c r="M19" t="inlineStr"/>
-    </row>
-    <row r="20">
-      <c r="A20" t="b">
-        <v>0</v>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>MEYTO Multi-Purpose/ E.C.</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>14.8833047964844</t>
-        </is>
-      </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>120.72904705443</t>
-        </is>
-      </c>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t>142</t>
-        </is>
-      </c>
-      <c r="F20" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="G20" t="inlineStr">
-        <is>
-          <t>284</t>
-        </is>
-      </c>
-      <c r="H20" t="inlineStr">
-        <is>
-          <t>8520000</t>
-        </is>
-      </c>
-      <c r="I20" t="inlineStr">
-        <is>
-          <t>True</t>
-        </is>
-      </c>
-      <c r="J20" t="inlineStr">
-        <is>
-          <t>True</t>
-        </is>
-      </c>
-      <c r="K20" t="inlineStr">
-        <is>
-          <t>True</t>
-        </is>
-      </c>
-      <c r="L20" t="inlineStr">
-        <is>
-          <t>Built</t>
-        </is>
-      </c>
-      <c r="M20" t="inlineStr"/>
-    </row>
-    <row r="21">
-      <c r="A21" t="b">
-        <v>0</v>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>Barangay Hall Bulusan</t>
-        </is>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>14.9087960788938</t>
-        </is>
-      </c>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>120.742261855893</t>
-        </is>
-      </c>
-      <c r="E21" t="inlineStr">
-        <is>
-          <t>700</t>
-        </is>
-      </c>
-      <c r="F21" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="G21" t="inlineStr">
-        <is>
-          <t>1400</t>
-        </is>
-      </c>
-      <c r="H21" t="inlineStr">
-        <is>
-          <t>42000000</t>
-        </is>
-      </c>
-      <c r="I21" t="inlineStr">
-        <is>
-          <t>True</t>
-        </is>
-      </c>
-      <c r="J21" t="inlineStr">
-        <is>
-          <t>True</t>
-        </is>
-      </c>
-      <c r="K21" t="inlineStr">
-        <is>
-          <t>True</t>
-        </is>
-      </c>
-      <c r="L21" t="inlineStr">
-        <is>
-          <t>Built</t>
-        </is>
-      </c>
-      <c r="M21" t="inlineStr"/>
-    </row>
-    <row r="22">
-      <c r="A22" t="b">
-        <v>0</v>
-      </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>Brgy. Hall Sta. Lucia</t>
-        </is>
-      </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>14.8995538574762</t>
-        </is>
-      </c>
-      <c r="D22" t="inlineStr">
-        <is>
-          <t>120.737428917917</t>
-        </is>
-      </c>
-      <c r="E22" t="inlineStr">
-        <is>
-          <t>150</t>
-        </is>
-      </c>
-      <c r="F22" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="G22" t="inlineStr">
-        <is>
-          <t>300</t>
-        </is>
-      </c>
-      <c r="H22" t="inlineStr">
-        <is>
-          <t>9000000</t>
-        </is>
-      </c>
-      <c r="I22" t="inlineStr">
-        <is>
-          <t>True</t>
-        </is>
-      </c>
-      <c r="J22" t="inlineStr">
-        <is>
-          <t>True</t>
-        </is>
-      </c>
-      <c r="K22" t="inlineStr">
-        <is>
-          <t>True</t>
-        </is>
-      </c>
-      <c r="L22" t="inlineStr">
-        <is>
-          <t>Built</t>
-        </is>
-      </c>
-      <c r="M22" t="inlineStr"/>
-    </row>
-    <row r="23">
-      <c r="A23" t="b">
-        <v>1</v>
-      </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>Mun. Covered Court</t>
-        </is>
-      </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>14.9141384055205</t>
-        </is>
-      </c>
-      <c r="D23" t="inlineStr">
-        <is>
-          <t>120.764788274642</t>
-        </is>
-      </c>
-      <c r="E23" t="inlineStr">
-        <is>
-          <t>713</t>
-        </is>
-      </c>
-      <c r="F23" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="G23" t="inlineStr">
-        <is>
-          <t>1426</t>
-        </is>
-      </c>
-      <c r="H23" t="inlineStr">
-        <is>
-          <t>42780000</t>
-        </is>
-      </c>
-      <c r="I23" t="inlineStr">
-        <is>
-          <t>True</t>
-        </is>
-      </c>
-      <c r="J23" t="inlineStr">
-        <is>
-          <t>True</t>
-        </is>
-      </c>
-      <c r="K23" t="inlineStr">
-        <is>
-          <t>True</t>
-        </is>
-      </c>
-      <c r="L23" t="inlineStr">
-        <is>
-          <t>Built</t>
-        </is>
-      </c>
-      <c r="M23" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>